<commit_message>
Change in usage phase methodology
</commit_message>
<xml_diff>
--- a/Grille_allocation_ab.xlsx
+++ b/Grille_allocation_ab.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louau\Projets\Ademe_RCP_FAI\modele-rcp-fai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F880A727-DF36-4AFB-A5AE-4C682B72EDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5C54CE-AD72-419D-ACD8-1971E4756D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t>Fabrication</t>
   </si>
@@ -297,6 +297,12 @@
   </si>
   <si>
     <t>Fibre optique 6 brins</t>
+  </si>
+  <si>
+    <t>Boucle locale cuivre</t>
+  </si>
+  <si>
+    <t>Boucle locale fibre</t>
   </si>
 </sst>
 </file>
@@ -852,7 +858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -999,6 +1005,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1008,32 +1074,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1041,84 +1128,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32657AA7-A293-41FC-8E8B-58993E82175E}">
-  <dimension ref="A1:AJ48"/>
+  <dimension ref="A1:AJ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AA35" sqref="AA35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1443,130 +1453,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="82" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="83"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="82" t="s">
+      <c r="N1" s="87"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="74"/>
-      <c r="AB1" s="74"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="74"/>
-      <c r="AF1" s="74"/>
-      <c r="AG1" s="74"/>
-      <c r="AH1" s="74"/>
-      <c r="AI1" s="74"/>
-      <c r="AJ1" s="75"/>
+      <c r="Z1" s="87"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="79"/>
     </row>
     <row r="2" spans="1:36" ht="26" x14ac:dyDescent="0.4">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="64" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="81"/>
+      <c r="E2" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66" t="s">
+      <c r="F2" s="92"/>
+      <c r="G2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="80" t="s">
+      <c r="H2" s="66"/>
+      <c r="I2" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="81"/>
-      <c r="K2" s="68" t="s">
+      <c r="J2" s="85"/>
+      <c r="K2" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="69"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="1"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="84" t="str">
+      <c r="O2" s="88" t="str">
         <f>C2</f>
         <v>Fabrication</v>
       </c>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="78" t="str">
+      <c r="P2" s="57"/>
+      <c r="Q2" s="82" t="str">
         <f>E2</f>
         <v>Distribution</v>
       </c>
-      <c r="R2" s="79"/>
-      <c r="S2" s="85" t="str">
+      <c r="R2" s="83"/>
+      <c r="S2" s="89" t="str">
         <f>G2</f>
         <v>Utilisation</v>
       </c>
-      <c r="T2" s="86"/>
-      <c r="U2" s="80" t="s">
+      <c r="T2" s="90"/>
+      <c r="U2" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="V2" s="81"/>
-      <c r="W2" s="68" t="str">
+      <c r="V2" s="85"/>
+      <c r="W2" s="67" t="str">
         <f>K2</f>
         <v>Fin de vie</v>
       </c>
-      <c r="X2" s="69"/>
+      <c r="X2" s="68"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="3"/>
-      <c r="AA2" s="58" t="str">
+      <c r="AA2" s="57" t="str">
         <f>O2</f>
         <v>Fabrication</v>
       </c>
-      <c r="AB2" s="58"/>
-      <c r="AC2" s="78" t="str">
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="82" t="str">
         <f>Q2</f>
         <v>Distribution</v>
       </c>
-      <c r="AD2" s="79"/>
-      <c r="AE2" s="85" t="str">
+      <c r="AD2" s="83"/>
+      <c r="AE2" s="89" t="str">
         <f>S2</f>
         <v>Utilisation</v>
       </c>
-      <c r="AF2" s="86"/>
-      <c r="AG2" s="80" t="s">
+      <c r="AF2" s="90"/>
+      <c r="AG2" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="AH2" s="81"/>
-      <c r="AI2" s="68" t="str">
+      <c r="AH2" s="85"/>
+      <c r="AI2" s="67" t="str">
         <f>W2</f>
         <v>Fin de vie</v>
       </c>
-      <c r="AJ2" s="69"/>
+      <c r="AJ2" s="68"/>
     </row>
     <row r="3" spans="1:36" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="55" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1699,7 +1709,7 @@
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="75" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="42" t="s">
@@ -1735,7 +1745,7 @@
       <c r="L4" s="32">
         <v>0</v>
       </c>
-      <c r="M4" s="70" t="s">
+      <c r="M4" s="69" t="s">
         <v>29</v>
       </c>
       <c r="N4" s="42" t="s">
@@ -1771,7 +1781,7 @@
       <c r="X4" s="19">
         <v>100</v>
       </c>
-      <c r="Y4" s="62" t="s">
+      <c r="Y4" s="58" t="s">
         <v>14</v>
       </c>
       <c r="Z4" s="42" t="s">
@@ -1809,7 +1819,7 @@
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A5" s="56"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="43" t="s">
         <v>19</v>
       </c>
@@ -1843,7 +1853,7 @@
       <c r="L5" s="17">
         <v>100</v>
       </c>
-      <c r="M5" s="71"/>
+      <c r="M5" s="70"/>
       <c r="N5" s="43" t="s">
         <v>32</v>
       </c>
@@ -1877,7 +1887,7 @@
       <c r="X5" s="17">
         <v>100</v>
       </c>
-      <c r="Y5" s="63"/>
+      <c r="Y5" s="59"/>
       <c r="Z5" s="43" t="s">
         <v>21</v>
       </c>
@@ -1913,7 +1923,7 @@
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A6" s="56"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="43" t="s">
         <v>22</v>
       </c>
@@ -1947,7 +1957,7 @@
       <c r="L6" s="17">
         <v>100</v>
       </c>
-      <c r="M6" s="71"/>
+      <c r="M6" s="70"/>
       <c r="N6" s="43" t="s">
         <v>35</v>
       </c>
@@ -1981,7 +1991,7 @@
       <c r="X6" s="17">
         <v>100</v>
       </c>
-      <c r="Y6" s="63"/>
+      <c r="Y6" s="59"/>
       <c r="Z6" s="43" t="s">
         <v>24</v>
       </c>
@@ -2017,7 +2027,7 @@
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A7" s="56"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="43" t="s">
         <v>25</v>
       </c>
@@ -2051,7 +2061,7 @@
       <c r="L7" s="17">
         <v>100</v>
       </c>
-      <c r="M7" s="71"/>
+      <c r="M7" s="70"/>
       <c r="N7" s="43" t="s">
         <v>38</v>
       </c>
@@ -2085,7 +2095,7 @@
       <c r="X7" s="17">
         <v>100</v>
       </c>
-      <c r="Y7" s="63"/>
+      <c r="Y7" s="59"/>
       <c r="Z7" s="43" t="s">
         <v>27</v>
       </c>
@@ -2121,7 +2131,7 @@
       </c>
     </row>
     <row r="8" spans="1:36" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="56"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="43" t="s">
         <v>28</v>
       </c>
@@ -2155,7 +2165,7 @@
       <c r="L8" s="17">
         <v>100</v>
       </c>
-      <c r="M8" s="71"/>
+      <c r="M8" s="70"/>
       <c r="N8" s="43" t="s">
         <v>41</v>
       </c>
@@ -2189,7 +2199,7 @@
       <c r="X8" s="17">
         <v>100</v>
       </c>
-      <c r="Y8" s="63"/>
+      <c r="Y8" s="59"/>
       <c r="Z8" s="43" t="s">
         <v>31</v>
       </c>
@@ -2225,7 +2235,7 @@
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A9" s="56"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="43" t="s">
         <v>7</v>
       </c>
@@ -2259,7 +2269,7 @@
       <c r="L9" s="17">
         <v>100</v>
       </c>
-      <c r="M9" s="71"/>
+      <c r="M9" s="70"/>
       <c r="N9" s="43" t="s">
         <v>44</v>
       </c>
@@ -2293,7 +2303,7 @@
       <c r="X9" s="17">
         <v>100</v>
       </c>
-      <c r="Y9" s="63"/>
+      <c r="Y9" s="59"/>
       <c r="Z9" s="43" t="s">
         <v>33</v>
       </c>
@@ -2329,7 +2339,7 @@
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A10" s="56"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="43" t="s">
         <v>34</v>
       </c>
@@ -2363,7 +2373,7 @@
       <c r="L10" s="17">
         <v>100</v>
       </c>
-      <c r="M10" s="71"/>
+      <c r="M10" s="70"/>
       <c r="N10" s="43" t="s">
         <v>47</v>
       </c>
@@ -2397,7 +2407,7 @@
       <c r="X10" s="17">
         <v>100</v>
       </c>
-      <c r="Y10" s="63"/>
+      <c r="Y10" s="59"/>
       <c r="Z10" s="43" t="s">
         <v>36</v>
       </c>
@@ -2433,7 +2443,7 @@
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A11" s="56"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="43" t="s">
         <v>37</v>
       </c>
@@ -2467,7 +2477,7 @@
       <c r="L11" s="17">
         <v>100</v>
       </c>
-      <c r="M11" s="71"/>
+      <c r="M11" s="70"/>
       <c r="N11" s="43" t="s">
         <v>50</v>
       </c>
@@ -2501,7 +2511,7 @@
       <c r="X11" s="17">
         <v>100</v>
       </c>
-      <c r="Y11" s="63"/>
+      <c r="Y11" s="59"/>
       <c r="Z11" s="43" t="s">
         <v>39</v>
       </c>
@@ -2537,7 +2547,7 @@
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A12" s="56"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="43" t="s">
         <v>40</v>
       </c>
@@ -2571,7 +2581,7 @@
       <c r="L12" s="17">
         <v>100</v>
       </c>
-      <c r="M12" s="72"/>
+      <c r="M12" s="71"/>
       <c r="N12" s="45" t="s">
         <v>53</v>
       </c>
@@ -2605,7 +2615,7 @@
       <c r="X12" s="17">
         <v>100</v>
       </c>
-      <c r="Y12" s="52" t="s">
+      <c r="Y12" s="72" t="s">
         <v>16</v>
       </c>
       <c r="Z12" s="44" t="s">
@@ -2643,7 +2653,7 @@
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A13" s="56"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="43" t="s">
         <v>43</v>
       </c>
@@ -2713,7 +2723,7 @@
       <c r="X13" s="21">
         <v>100</v>
       </c>
-      <c r="Y13" s="53"/>
+      <c r="Y13" s="73"/>
       <c r="Z13" s="43" t="s">
         <v>17</v>
       </c>
@@ -2749,7 +2759,7 @@
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A14" s="56"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="43" t="s">
         <v>85</v>
       </c>
@@ -2819,7 +2829,7 @@
       <c r="X14" s="21">
         <v>100</v>
       </c>
-      <c r="Y14" s="54"/>
+      <c r="Y14" s="74"/>
       <c r="Z14" s="45" t="s">
         <v>20</v>
       </c>
@@ -2855,7 +2865,7 @@
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A15" s="56"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="43" t="s">
         <v>86</v>
       </c>
@@ -2925,7 +2935,7 @@
       <c r="X15" s="21">
         <v>100</v>
       </c>
-      <c r="Y15" s="52" t="s">
+      <c r="Y15" s="72" t="s">
         <v>23</v>
       </c>
       <c r="Z15" s="44" t="s">
@@ -2963,44 +2973,53 @@
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A16" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="30">
-        <v>100</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12">
-        <v>100</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="A16" s="61"/>
+      <c r="B16" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="16">
+        <v>100</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <v>100</v>
+      </c>
+      <c r="G16" s="16">
         <v>20</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="16">
         <v>80</v>
       </c>
-      <c r="I16" s="12">
-        <v>100</v>
-      </c>
-      <c r="J16" s="12">
-        <v>0</v>
-      </c>
-      <c r="K16" s="12">
-        <v>100</v>
-      </c>
-      <c r="L16" s="19">
-        <v>0</v>
-      </c>
-      <c r="N16" s="23"/>
-      <c r="Y16" s="53"/>
+      <c r="I16" s="16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="16">
+        <v>100</v>
+      </c>
+      <c r="K16" s="16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="17">
+        <v>100</v>
+      </c>
+      <c r="M16" s="56"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="73"/>
       <c r="Z16" s="43" t="s">
         <v>26</v>
       </c>
@@ -3036,42 +3055,53 @@
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A17" s="60"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0</v>
+      </c>
+      <c r="D17" s="16">
+        <v>100</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0</v>
+      </c>
+      <c r="F17" s="16">
+        <v>100</v>
+      </c>
+      <c r="G17" s="16">
         <v>20</v>
       </c>
-      <c r="C17" s="33">
-        <v>100</v>
-      </c>
-      <c r="D17" s="13">
-        <v>0</v>
-      </c>
-      <c r="E17" s="13">
-        <v>100</v>
-      </c>
-      <c r="F17" s="13">
-        <v>0</v>
-      </c>
-      <c r="G17" s="13">
-        <v>20</v>
-      </c>
-      <c r="H17" s="13">
+      <c r="H17" s="16">
         <v>80</v>
       </c>
-      <c r="I17" s="13">
-        <v>100</v>
-      </c>
-      <c r="J17" s="13">
-        <v>0</v>
-      </c>
-      <c r="K17" s="13">
-        <v>100</v>
-      </c>
-      <c r="L17" s="18">
-        <v>0</v>
-      </c>
-      <c r="N17" s="22"/>
-      <c r="Y17" s="53"/>
+      <c r="I17" s="16">
+        <v>0</v>
+      </c>
+      <c r="J17" s="16">
+        <v>100</v>
+      </c>
+      <c r="K17" s="16">
+        <v>0</v>
+      </c>
+      <c r="L17" s="17">
+        <v>100</v>
+      </c>
+      <c r="M17" s="56"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="73"/>
       <c r="Z17" s="50" t="s">
         <v>45</v>
       </c>
@@ -3107,54 +3137,44 @@
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A18" s="59" t="s">
-        <v>23</v>
+      <c r="A18" s="63" t="s">
+        <v>16</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="16">
-        <v>100</v>
-      </c>
-      <c r="D18" s="16">
-        <v>0</v>
-      </c>
-      <c r="E18" s="16">
-        <v>100</v>
-      </c>
-      <c r="F18" s="16">
-        <v>0</v>
-      </c>
-      <c r="G18" s="16">
+        <v>17</v>
+      </c>
+      <c r="C18" s="30">
+        <v>100</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12">
+        <v>100</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
         <v>20</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="12">
         <v>80</v>
       </c>
-      <c r="I18" s="16">
-        <v>100</v>
-      </c>
-      <c r="J18" s="16">
-        <v>0</v>
-      </c>
-      <c r="K18" s="16">
-        <v>100</v>
-      </c>
-      <c r="L18" s="17">
+      <c r="I18" s="12">
+        <v>100</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <v>100</v>
+      </c>
+      <c r="L18" s="19">
         <v>0</v>
       </c>
       <c r="N18" s="22"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="17"/>
-      <c r="Y18" s="53"/>
+      <c r="Y18" s="73"/>
       <c r="Z18" s="43" t="s">
         <v>48</v>
       </c>
@@ -3190,52 +3210,42 @@
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A19" s="60"/>
-      <c r="B19" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="16">
-        <v>100</v>
-      </c>
-      <c r="D19" s="16">
-        <v>0</v>
-      </c>
-      <c r="E19" s="16">
-        <v>100</v>
-      </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-      <c r="G19" s="16">
+      <c r="A19" s="64"/>
+      <c r="B19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="16">
+      <c r="C19" s="33">
+        <v>100</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0</v>
+      </c>
+      <c r="E19" s="13">
+        <v>100</v>
+      </c>
+      <c r="F19" s="13">
+        <v>0</v>
+      </c>
+      <c r="G19" s="13">
+        <v>20</v>
+      </c>
+      <c r="H19" s="13">
         <v>80</v>
       </c>
-      <c r="I19" s="16">
-        <v>100</v>
-      </c>
-      <c r="J19" s="16">
-        <v>0</v>
-      </c>
-      <c r="K19" s="16">
-        <v>100</v>
-      </c>
-      <c r="L19" s="17">
+      <c r="I19" s="13">
+        <v>100</v>
+      </c>
+      <c r="J19" s="13">
+        <v>0</v>
+      </c>
+      <c r="K19" s="13">
+        <v>100</v>
+      </c>
+      <c r="L19" s="18">
         <v>0</v>
       </c>
       <c r="N19" s="22"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="16"/>
-      <c r="X19" s="17"/>
-      <c r="Y19" s="53"/>
+      <c r="Y19" s="73"/>
       <c r="Z19" s="43" t="s">
         <v>51</v>
       </c>
@@ -3271,41 +3281,41 @@
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A20" s="55" t="s">
-        <v>46</v>
+      <c r="A20" s="63" t="s">
+        <v>23</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="12">
-        <v>0</v>
-      </c>
-      <c r="D20" s="12">
-        <v>100</v>
-      </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12">
-        <v>100</v>
-      </c>
-      <c r="G20" s="12">
-        <v>0</v>
-      </c>
-      <c r="H20" s="12">
-        <v>100</v>
-      </c>
-      <c r="I20" s="12">
-        <v>0</v>
-      </c>
-      <c r="J20" s="12">
-        <v>100</v>
-      </c>
-      <c r="K20" s="12">
-        <v>0</v>
-      </c>
-      <c r="L20" s="19">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="C20" s="16">
+        <v>100</v>
+      </c>
+      <c r="D20" s="16">
+        <v>0</v>
+      </c>
+      <c r="E20" s="16">
+        <v>100</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0</v>
+      </c>
+      <c r="G20" s="16">
+        <v>20</v>
+      </c>
+      <c r="H20" s="16">
+        <v>80</v>
+      </c>
+      <c r="I20" s="16">
+        <v>100</v>
+      </c>
+      <c r="J20" s="16">
+        <v>0</v>
+      </c>
+      <c r="K20" s="16">
+        <v>100</v>
+      </c>
+      <c r="L20" s="17">
+        <v>0</v>
       </c>
       <c r="N20" s="22"/>
       <c r="O20" s="16"/>
@@ -3318,7 +3328,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="17"/>
-      <c r="Y20" s="53"/>
+      <c r="Y20" s="73"/>
       <c r="Z20" s="43" t="s">
         <v>54</v>
       </c>
@@ -3354,39 +3364,39 @@
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A21" s="56"/>
-      <c r="B21" s="46" t="s">
-        <v>49</v>
+      <c r="A21" s="64"/>
+      <c r="B21" s="45" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="16">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D21" s="16">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E21" s="16">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F21" s="16">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G21" s="16">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H21" s="16">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I21" s="16">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J21" s="16">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K21" s="16">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L21" s="17">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N21" s="22"/>
       <c r="O21" s="16"/>
@@ -3399,7 +3409,7 @@
       <c r="V21" s="16"/>
       <c r="W21" s="16"/>
       <c r="X21" s="17"/>
-      <c r="Y21" s="53"/>
+      <c r="Y21" s="73"/>
       <c r="Z21" s="43" t="s">
         <v>57</v>
       </c>
@@ -3435,38 +3445,40 @@
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A22" s="57"/>
-      <c r="B22" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="13">
-        <v>0</v>
-      </c>
-      <c r="D22" s="13">
-        <v>100</v>
-      </c>
-      <c r="E22" s="13">
-        <v>0</v>
-      </c>
-      <c r="F22" s="13">
-        <v>100</v>
-      </c>
-      <c r="G22" s="13">
-        <v>0</v>
-      </c>
-      <c r="H22" s="13">
-        <v>100</v>
-      </c>
-      <c r="I22" s="13">
-        <v>0</v>
-      </c>
-      <c r="J22" s="13">
-        <v>100</v>
-      </c>
-      <c r="K22" s="13">
-        <v>0</v>
-      </c>
-      <c r="L22" s="18">
+      <c r="A22" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>100</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>100</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>100</v>
+      </c>
+      <c r="I22" s="12">
+        <v>0</v>
+      </c>
+      <c r="J22" s="12">
+        <v>100</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="19">
         <v>100</v>
       </c>
       <c r="N22" s="22"/>
@@ -3480,7 +3492,7 @@
       <c r="V22" s="16"/>
       <c r="W22" s="16"/>
       <c r="X22" s="17"/>
-      <c r="Y22" s="54"/>
+      <c r="Y22" s="74"/>
       <c r="Z22" s="45" t="s">
         <v>59</v>
       </c>
@@ -3516,40 +3528,38 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A23" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="12">
-        <v>0</v>
-      </c>
-      <c r="D23" s="12">
-        <v>100</v>
-      </c>
-      <c r="E23" s="12">
-        <v>0</v>
-      </c>
-      <c r="F23" s="12">
-        <v>100</v>
-      </c>
-      <c r="G23" s="12">
-        <v>0</v>
-      </c>
-      <c r="H23" s="12">
-        <v>100</v>
-      </c>
-      <c r="I23" s="12">
-        <v>0</v>
-      </c>
-      <c r="J23" s="12">
-        <v>100</v>
-      </c>
-      <c r="K23" s="12">
-        <v>0</v>
-      </c>
-      <c r="L23" s="19">
+      <c r="A23" s="61"/>
+      <c r="B23" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0</v>
+      </c>
+      <c r="D23" s="16">
+        <v>100</v>
+      </c>
+      <c r="E23" s="16">
+        <v>0</v>
+      </c>
+      <c r="F23" s="16">
+        <v>100</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+      <c r="H23" s="16">
+        <v>100</v>
+      </c>
+      <c r="I23" s="16">
+        <v>0</v>
+      </c>
+      <c r="J23" s="16">
+        <v>100</v>
+      </c>
+      <c r="K23" s="16">
+        <v>0</v>
+      </c>
+      <c r="L23" s="17">
         <v>100</v>
       </c>
       <c r="N23" s="22"/>
@@ -3563,7 +3573,7 @@
       <c r="V23" s="16"/>
       <c r="W23" s="16"/>
       <c r="X23" s="17"/>
-      <c r="Y23" s="55" t="s">
+      <c r="Y23" s="60" t="s">
         <v>60</v>
       </c>
       <c r="Z23" s="43" t="s">
@@ -3600,39 +3610,39 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A24" s="56"/>
-      <c r="B24" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="16">
-        <v>0</v>
-      </c>
-      <c r="D24" s="16">
-        <v>100</v>
-      </c>
-      <c r="E24" s="16">
-        <v>0</v>
-      </c>
-      <c r="F24" s="16">
-        <v>100</v>
-      </c>
-      <c r="G24" s="16">
-        <v>0</v>
-      </c>
-      <c r="H24" s="16">
-        <v>100</v>
-      </c>
-      <c r="I24" s="16">
-        <v>0</v>
-      </c>
-      <c r="J24" s="16">
-        <v>100</v>
-      </c>
-      <c r="K24" s="16">
-        <v>0</v>
-      </c>
-      <c r="L24" s="17">
+    <row r="24" spans="1:36" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="62"/>
+      <c r="B24" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0</v>
+      </c>
+      <c r="D24" s="13">
+        <v>100</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0</v>
+      </c>
+      <c r="F24" s="13">
+        <v>100</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <v>100</v>
+      </c>
+      <c r="I24" s="13">
+        <v>0</v>
+      </c>
+      <c r="J24" s="13">
+        <v>100</v>
+      </c>
+      <c r="K24" s="13">
+        <v>0</v>
+      </c>
+      <c r="L24" s="18">
         <v>100</v>
       </c>
       <c r="N24" s="22"/>
@@ -3646,7 +3656,7 @@
       <c r="V24" s="16"/>
       <c r="W24" s="16"/>
       <c r="X24" s="17"/>
-      <c r="Y24" s="56"/>
+      <c r="Y24" s="61"/>
       <c r="Z24" s="46" t="s">
         <v>62</v>
       </c>
@@ -3682,42 +3692,43 @@
       </c>
     </row>
     <row r="25" spans="1:36" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="56"/>
-      <c r="B25" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="16">
-        <v>0</v>
-      </c>
-      <c r="D25" s="16">
-        <v>100</v>
-      </c>
-      <c r="E25" s="16">
-        <v>0</v>
-      </c>
-      <c r="F25" s="16">
-        <v>100</v>
-      </c>
-      <c r="G25" s="16">
-        <v>0</v>
-      </c>
-      <c r="H25" s="16">
-        <v>100</v>
-      </c>
-      <c r="I25" s="16">
-        <v>0</v>
-      </c>
-      <c r="J25" s="16">
-        <v>100</v>
-      </c>
-      <c r="K25" s="16">
-        <v>0</v>
-      </c>
-      <c r="L25" s="17">
-        <v>100</v>
-      </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="24"/>
+      <c r="A25" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0</v>
+      </c>
+      <c r="D25" s="12">
+        <v>100</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>100</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <v>100</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0</v>
+      </c>
+      <c r="J25" s="12">
+        <v>100</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="19">
+        <v>100</v>
+      </c>
+      <c r="N25" s="22"/>
       <c r="O25" s="16"/>
       <c r="P25" s="16"/>
       <c r="Q25" s="16"/>
@@ -3728,7 +3739,7 @@
       <c r="V25" s="16"/>
       <c r="W25" s="16"/>
       <c r="X25" s="17"/>
-      <c r="Y25" s="56"/>
+      <c r="Y25" s="61"/>
       <c r="Z25" s="46" t="s">
         <v>64</v>
       </c>
@@ -3764,9 +3775,9 @@
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A26" s="56"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="46" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C26" s="16">
         <v>0</v>
@@ -3798,8 +3809,7 @@
       <c r="L26" s="17">
         <v>100</v>
       </c>
-      <c r="M26" s="38"/>
-      <c r="N26" s="24"/>
+      <c r="N26" s="22"/>
       <c r="O26" s="16"/>
       <c r="P26" s="16"/>
       <c r="Q26" s="16"/>
@@ -3810,7 +3820,7 @@
       <c r="V26" s="16"/>
       <c r="W26" s="16"/>
       <c r="X26" s="17"/>
-      <c r="Y26" s="56"/>
+      <c r="Y26" s="61"/>
       <c r="Z26" s="51" t="s">
         <v>66</v>
       </c>
@@ -3845,10 +3855,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A27" s="56"/>
+    <row r="27" spans="1:36" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="61"/>
       <c r="B27" s="46" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C27" s="16">
         <v>0</v>
@@ -3880,7 +3890,7 @@
       <c r="L27" s="17">
         <v>100</v>
       </c>
-      <c r="M27" s="38"/>
+      <c r="M27" s="16"/>
       <c r="N27" s="24"/>
       <c r="O27" s="16"/>
       <c r="P27" s="16"/>
@@ -3892,7 +3902,7 @@
       <c r="V27" s="16"/>
       <c r="W27" s="16"/>
       <c r="X27" s="17"/>
-      <c r="Y27" s="57"/>
+      <c r="Y27" s="62"/>
       <c r="Z27" s="51" t="s">
         <v>68</v>
       </c>
@@ -3928,9 +3938,9 @@
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A28" s="56"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C28" s="16">
         <v>0</v>
@@ -3974,7 +3984,7 @@
       <c r="V28" s="16"/>
       <c r="W28" s="16"/>
       <c r="X28" s="17"/>
-      <c r="Y28" s="55" t="s">
+      <c r="Y28" s="60" t="s">
         <v>80</v>
       </c>
       <c r="Z28" s="44" t="s">
@@ -4012,9 +4022,9 @@
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A29" s="56"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="46" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C29" s="16">
         <v>0</v>
@@ -4058,7 +4068,7 @@
       <c r="V29" s="16"/>
       <c r="W29" s="16"/>
       <c r="X29" s="17"/>
-      <c r="Y29" s="56"/>
+      <c r="Y29" s="61"/>
       <c r="Z29" s="46" t="s">
         <v>62</v>
       </c>
@@ -4094,9 +4104,9 @@
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A30" s="56"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C30" s="16">
         <v>0</v>
@@ -4140,7 +4150,7 @@
       <c r="V30" s="16"/>
       <c r="W30" s="16"/>
       <c r="X30" s="17"/>
-      <c r="Y30" s="57"/>
+      <c r="Y30" s="62"/>
       <c r="Z30" s="47" t="s">
         <v>64</v>
       </c>
@@ -4176,9 +4186,9 @@
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A31" s="56"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="46" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" s="16">
         <v>0</v>
@@ -4222,7 +4232,7 @@
       <c r="V31" s="16"/>
       <c r="W31" s="16"/>
       <c r="X31" s="17"/>
-      <c r="Y31" s="55" t="s">
+      <c r="Y31" s="60" t="s">
         <v>83</v>
       </c>
       <c r="Z31" s="44" t="s">
@@ -4260,9 +4270,9 @@
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A32" s="56"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C32" s="16">
         <v>0</v>
@@ -4306,7 +4316,7 @@
       <c r="V32" s="16"/>
       <c r="W32" s="16"/>
       <c r="X32" s="17"/>
-      <c r="Y32" s="56"/>
+      <c r="Y32" s="61"/>
       <c r="Z32" s="46" t="s">
         <v>62</v>
       </c>
@@ -4342,41 +4352,41 @@
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A33" s="57"/>
-      <c r="B33" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="13">
-        <v>0</v>
-      </c>
-      <c r="D33" s="13">
-        <v>100</v>
-      </c>
-      <c r="E33" s="13">
-        <v>0</v>
-      </c>
-      <c r="F33" s="13">
-        <v>100</v>
-      </c>
-      <c r="G33" s="13">
-        <v>0</v>
-      </c>
-      <c r="H33" s="13">
-        <v>100</v>
-      </c>
-      <c r="I33" s="13">
-        <v>0</v>
-      </c>
-      <c r="J33" s="13">
-        <v>100</v>
-      </c>
-      <c r="K33" s="13">
-        <v>0</v>
-      </c>
-      <c r="L33" s="18">
-        <v>100</v>
-      </c>
-      <c r="M33" s="16"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="16">
+        <v>0</v>
+      </c>
+      <c r="D33" s="16">
+        <v>100</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0</v>
+      </c>
+      <c r="F33" s="16">
+        <v>100</v>
+      </c>
+      <c r="G33" s="16">
+        <v>0</v>
+      </c>
+      <c r="H33" s="16">
+        <v>100</v>
+      </c>
+      <c r="I33" s="16">
+        <v>0</v>
+      </c>
+      <c r="J33" s="16">
+        <v>100</v>
+      </c>
+      <c r="K33" s="16">
+        <v>0</v>
+      </c>
+      <c r="L33" s="17">
+        <v>100</v>
+      </c>
+      <c r="M33" s="38"/>
       <c r="N33" s="24"/>
       <c r="O33" s="16"/>
       <c r="P33" s="16"/>
@@ -4388,8 +4398,8 @@
       <c r="V33" s="16"/>
       <c r="W33" s="16"/>
       <c r="X33" s="17"/>
-      <c r="Y33" s="57"/>
-      <c r="Z33" s="47" t="s">
+      <c r="Y33" s="62"/>
+      <c r="Z33" s="46" t="s">
         <v>64</v>
       </c>
       <c r="AA33" s="13">
@@ -4424,11 +4434,9 @@
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A34" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>73</v>
+      <c r="A34" s="61"/>
+      <c r="B34" s="46" t="s">
+        <v>70</v>
       </c>
       <c r="C34" s="16">
         <v>0</v>
@@ -4460,7 +4468,7 @@
       <c r="L34" s="17">
         <v>100</v>
       </c>
-      <c r="M34" s="16"/>
+      <c r="M34" s="38"/>
       <c r="N34" s="24"/>
       <c r="O34" s="16"/>
       <c r="P34" s="16"/>
@@ -4472,43 +4480,41 @@
       <c r="V34" s="16"/>
       <c r="W34" s="16"/>
       <c r="X34" s="17"/>
-      <c r="Y34" s="36"/>
       <c r="Z34" s="23"/>
-      <c r="AJ34" s="37"/>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A35" s="56"/>
-      <c r="B35" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="16">
-        <v>0</v>
-      </c>
-      <c r="D35" s="16">
-        <v>100</v>
-      </c>
-      <c r="E35" s="16">
-        <v>0</v>
-      </c>
-      <c r="F35" s="16">
-        <v>100</v>
-      </c>
-      <c r="G35" s="16">
-        <v>0</v>
-      </c>
-      <c r="H35" s="16">
-        <v>100</v>
-      </c>
-      <c r="I35" s="16">
-        <v>0</v>
-      </c>
-      <c r="J35" s="16">
-        <v>100</v>
-      </c>
-      <c r="K35" s="16">
-        <v>0</v>
-      </c>
-      <c r="L35" s="17">
+      <c r="A35" s="62"/>
+      <c r="B35" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="13">
+        <v>0</v>
+      </c>
+      <c r="D35" s="13">
+        <v>100</v>
+      </c>
+      <c r="E35" s="13">
+        <v>0</v>
+      </c>
+      <c r="F35" s="13">
+        <v>100</v>
+      </c>
+      <c r="G35" s="13">
+        <v>0</v>
+      </c>
+      <c r="H35" s="13">
+        <v>100</v>
+      </c>
+      <c r="I35" s="13">
+        <v>0</v>
+      </c>
+      <c r="J35" s="13">
+        <v>100</v>
+      </c>
+      <c r="K35" s="13">
+        <v>0</v>
+      </c>
+      <c r="L35" s="18">
         <v>100</v>
       </c>
       <c r="M35" s="16"/>
@@ -4523,14 +4529,14 @@
       <c r="V35" s="16"/>
       <c r="W35" s="16"/>
       <c r="X35" s="17"/>
-      <c r="Y35" s="36"/>
-      <c r="Z35" s="22"/>
-      <c r="AJ35" s="37"/>
+      <c r="Z35" s="93"/>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A36" s="56"/>
-      <c r="B36" s="46" t="s">
-        <v>52</v>
+      <c r="A36" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>73</v>
       </c>
       <c r="C36" s="16">
         <v>0</v>
@@ -4574,23 +4580,14 @@
       <c r="V36" s="16"/>
       <c r="W36" s="16"/>
       <c r="X36" s="17"/>
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="24"/>
-      <c r="AA36" s="16"/>
-      <c r="AB36" s="16"/>
-      <c r="AC36" s="16"/>
-      <c r="AD36" s="16"/>
-      <c r="AE36" s="16"/>
-      <c r="AF36" s="16"/>
-      <c r="AG36" s="16"/>
-      <c r="AH36" s="16"/>
-      <c r="AI36" s="16"/>
-      <c r="AJ36" s="17"/>
+      <c r="Y36" s="36"/>
+      <c r="Z36" s="22"/>
+      <c r="AJ36" s="37"/>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A37" s="56"/>
+      <c r="A37" s="61"/>
       <c r="B37" s="46" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C37" s="16">
         <v>0</v>
@@ -4634,23 +4631,14 @@
       <c r="V37" s="16"/>
       <c r="W37" s="16"/>
       <c r="X37" s="17"/>
-      <c r="Y37" s="25"/>
-      <c r="Z37" s="24"/>
-      <c r="AA37" s="16"/>
-      <c r="AB37" s="16"/>
-      <c r="AC37" s="16"/>
-      <c r="AD37" s="16"/>
-      <c r="AE37" s="16"/>
-      <c r="AF37" s="16"/>
-      <c r="AG37" s="16"/>
-      <c r="AH37" s="16"/>
-      <c r="AI37" s="16"/>
-      <c r="AJ37" s="17"/>
+      <c r="Y37" s="36"/>
+      <c r="Z37" s="22"/>
+      <c r="AJ37" s="37"/>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A38" s="56"/>
+      <c r="A38" s="61"/>
       <c r="B38" s="46" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C38" s="16">
         <v>0</v>
@@ -4708,9 +4696,9 @@
       <c r="AJ38" s="17"/>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A39" s="56"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C39" s="16">
         <v>0</v>
@@ -4768,9 +4756,9 @@
       <c r="AJ39" s="17"/>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A40" s="56"/>
+      <c r="A40" s="61"/>
       <c r="B40" s="46" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C40" s="16">
         <v>0</v>
@@ -4828,9 +4816,9 @@
       <c r="AJ40" s="17"/>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A41" s="56"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C41" s="16">
         <v>0</v>
@@ -4888,9 +4876,9 @@
       <c r="AJ41" s="17"/>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A42" s="56"/>
+      <c r="A42" s="61"/>
       <c r="B42" s="46" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C42" s="16">
         <v>0</v>
@@ -4948,9 +4936,9 @@
       <c r="AJ42" s="17"/>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A43" s="56"/>
+      <c r="A43" s="61"/>
       <c r="B43" s="46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C43" s="16">
         <v>0</v>
@@ -5008,9 +4996,9 @@
       <c r="AJ43" s="17"/>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A44" s="56"/>
+      <c r="A44" s="61"/>
       <c r="B44" s="46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C44" s="16">
         <v>0</v>
@@ -5068,9 +5056,9 @@
       <c r="AJ44" s="17"/>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A45" s="56"/>
+      <c r="A45" s="61"/>
       <c r="B45" s="46" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C45" s="16">
         <v>0</v>
@@ -5128,9 +5116,9 @@
       <c r="AJ45" s="17"/>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A46" s="56"/>
+      <c r="A46" s="61"/>
       <c r="B46" s="46" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C46" s="16">
         <v>0</v>
@@ -5188,9 +5176,9 @@
       <c r="AJ46" s="17"/>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A47" s="56"/>
+      <c r="A47" s="61"/>
       <c r="B47" s="46" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C47" s="16">
         <v>0</v>
@@ -5247,69 +5235,193 @@
       <c r="AI47" s="16"/>
       <c r="AJ47" s="17"/>
     </row>
-    <row r="48" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="87"/>
-      <c r="B48" s="48" t="s">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A48" s="61"/>
+      <c r="B48" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="16">
+        <v>0</v>
+      </c>
+      <c r="D48" s="16">
+        <v>100</v>
+      </c>
+      <c r="E48" s="16">
+        <v>0</v>
+      </c>
+      <c r="F48" s="16">
+        <v>100</v>
+      </c>
+      <c r="G48" s="16">
+        <v>0</v>
+      </c>
+      <c r="H48" s="16">
+        <v>100</v>
+      </c>
+      <c r="I48" s="16">
+        <v>0</v>
+      </c>
+      <c r="J48" s="16">
+        <v>100</v>
+      </c>
+      <c r="K48" s="16">
+        <v>0</v>
+      </c>
+      <c r="L48" s="17">
+        <v>100</v>
+      </c>
+      <c r="M48" s="16"/>
+      <c r="N48" s="24"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="16"/>
+      <c r="S48" s="16"/>
+      <c r="T48" s="16"/>
+      <c r="U48" s="16"/>
+      <c r="V48" s="16"/>
+      <c r="W48" s="16"/>
+      <c r="X48" s="17"/>
+      <c r="Y48" s="25"/>
+      <c r="Z48" s="24"/>
+      <c r="AA48" s="16"/>
+      <c r="AB48" s="16"/>
+      <c r="AC48" s="16"/>
+      <c r="AD48" s="16"/>
+      <c r="AE48" s="16"/>
+      <c r="AF48" s="16"/>
+      <c r="AG48" s="16"/>
+      <c r="AH48" s="16"/>
+      <c r="AI48" s="16"/>
+      <c r="AJ48" s="17"/>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A49" s="61"/>
+      <c r="B49" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="16">
+        <v>0</v>
+      </c>
+      <c r="D49" s="16">
+        <v>100</v>
+      </c>
+      <c r="E49" s="16">
+        <v>0</v>
+      </c>
+      <c r="F49" s="16">
+        <v>100</v>
+      </c>
+      <c r="G49" s="16">
+        <v>0</v>
+      </c>
+      <c r="H49" s="16">
+        <v>100</v>
+      </c>
+      <c r="I49" s="16">
+        <v>0</v>
+      </c>
+      <c r="J49" s="16">
+        <v>100</v>
+      </c>
+      <c r="K49" s="16">
+        <v>0</v>
+      </c>
+      <c r="L49" s="17">
+        <v>100</v>
+      </c>
+      <c r="M49" s="16"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="16"/>
+      <c r="T49" s="16"/>
+      <c r="U49" s="16"/>
+      <c r="V49" s="16"/>
+      <c r="W49" s="16"/>
+      <c r="X49" s="17"/>
+      <c r="Y49" s="25"/>
+      <c r="Z49" s="24"/>
+      <c r="AA49" s="16"/>
+      <c r="AB49" s="16"/>
+      <c r="AC49" s="16"/>
+      <c r="AD49" s="16"/>
+      <c r="AE49" s="16"/>
+      <c r="AF49" s="16"/>
+      <c r="AG49" s="16"/>
+      <c r="AH49" s="16"/>
+      <c r="AI49" s="16"/>
+      <c r="AJ49" s="17"/>
+    </row>
+    <row r="50" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="76"/>
+      <c r="B50" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="20">
-        <v>0</v>
-      </c>
-      <c r="D48" s="20">
-        <v>100</v>
-      </c>
-      <c r="E48" s="20">
-        <v>0</v>
-      </c>
-      <c r="F48" s="20">
-        <v>100</v>
-      </c>
-      <c r="G48" s="20">
-        <v>0</v>
-      </c>
-      <c r="H48" s="20">
-        <v>100</v>
-      </c>
-      <c r="I48" s="20">
-        <v>0</v>
-      </c>
-      <c r="J48" s="20">
-        <v>100</v>
-      </c>
-      <c r="K48" s="20">
-        <v>0</v>
-      </c>
-      <c r="L48" s="26">
-        <v>100</v>
-      </c>
-      <c r="M48" s="20"/>
-      <c r="N48" s="28"/>
-      <c r="O48" s="20"/>
-      <c r="P48" s="20"/>
-      <c r="Q48" s="20"/>
-      <c r="R48" s="20"/>
-      <c r="S48" s="20"/>
-      <c r="T48" s="20"/>
-      <c r="U48" s="20"/>
-      <c r="V48" s="20"/>
-      <c r="W48" s="20"/>
-      <c r="X48" s="26"/>
-      <c r="Y48" s="27"/>
-      <c r="Z48" s="28"/>
-      <c r="AA48" s="20"/>
-      <c r="AB48" s="20"/>
-      <c r="AC48" s="20"/>
-      <c r="AD48" s="20"/>
-      <c r="AE48" s="20"/>
-      <c r="AF48" s="20"/>
-      <c r="AG48" s="20"/>
-      <c r="AH48" s="20"/>
-      <c r="AI48" s="20"/>
-      <c r="AJ48" s="26"/>
+      <c r="C50" s="20">
+        <v>0</v>
+      </c>
+      <c r="D50" s="20">
+        <v>100</v>
+      </c>
+      <c r="E50" s="20">
+        <v>0</v>
+      </c>
+      <c r="F50" s="20">
+        <v>100</v>
+      </c>
+      <c r="G50" s="20">
+        <v>0</v>
+      </c>
+      <c r="H50" s="20">
+        <v>100</v>
+      </c>
+      <c r="I50" s="20">
+        <v>0</v>
+      </c>
+      <c r="J50" s="20">
+        <v>100</v>
+      </c>
+      <c r="K50" s="20">
+        <v>0</v>
+      </c>
+      <c r="L50" s="26">
+        <v>100</v>
+      </c>
+      <c r="M50" s="20"/>
+      <c r="N50" s="28"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="20"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="20"/>
+      <c r="S50" s="20"/>
+      <c r="T50" s="20"/>
+      <c r="U50" s="20"/>
+      <c r="V50" s="20"/>
+      <c r="W50" s="20"/>
+      <c r="X50" s="26"/>
+      <c r="Y50" s="27"/>
+      <c r="Z50" s="28"/>
+      <c r="AA50" s="20"/>
+      <c r="AB50" s="20"/>
+      <c r="AC50" s="20"/>
+      <c r="AD50" s="20"/>
+      <c r="AE50" s="20"/>
+      <c r="AF50" s="20"/>
+      <c r="AG50" s="20"/>
+      <c r="AH50" s="20"/>
+      <c r="AI50" s="20"/>
+      <c r="AJ50" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A34:A48"/>
+    <mergeCell ref="Y23:Y27"/>
+    <mergeCell ref="Y15:Y22"/>
+    <mergeCell ref="Y31:Y33"/>
+    <mergeCell ref="Y28:Y30"/>
+    <mergeCell ref="A36:A50"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="AC2:AD2"/>
@@ -5325,21 +5437,17 @@
     <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="AG2:AH2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M4:M12"/>
     <mergeCell ref="Y12:Y14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A33"/>
-    <mergeCell ref="A4:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="Y15:Y22"/>
-    <mergeCell ref="Y23:Y27"/>
-    <mergeCell ref="Y28:Y30"/>
-    <mergeCell ref="Y31:Y33"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A4:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>